<commit_message>
Update Optica BAC-17-Componente motivacional.xlsx
</commit_message>
<xml_diff>
--- a/HT-6/Optica BAC-17-Componente motivacional.xlsx
+++ b/HT-6/Optica BAC-17-Componente motivacional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juan/Documents/Universidad/2022-20/arquiemp/repo/arquiemp/HT-6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C17375-4A88-1745-9372-C220803E46A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27FF4CB3-EDC0-5C4F-A89F-335972A81374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1320" yWindow="500" windowWidth="17440" windowHeight="14920" xr2:uid="{6D2ADF59-F33A-44E3-88FB-8431094B32CC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Descripción</t>
   </si>
@@ -75,9 +75,6 @@
     <t>Óptica el mundo de las gafas</t>
   </si>
   <si>
-    <t>Permitirle a todos nuestros clientes tener una visión clara del mundo que los rodea.</t>
-  </si>
-  <si>
     <t>Para el 2030 llegar a 100 ópticas abiertas a nivel nacional.</t>
   </si>
   <si>
@@ -94,6 +91,45 @@
   </si>
   <si>
     <t>v5</t>
+  </si>
+  <si>
+    <t>Ser la marca de óptica reconocida y preferida por los colombianos.</t>
+  </si>
+  <si>
+    <t>Queremos brindar visión a nuestros clientes, porque ver el mundo te ayuda a comprenderlo.</t>
+  </si>
+  <si>
+    <t>Nuestra misión es ofrecer monturas y lentes de calidad a precios razonables, con diseños característicos y elegantes, que usen materiales resistentes y que sean reconocibles.</t>
+  </si>
+  <si>
+    <t>Responsabilidad ambiental</t>
+  </si>
+  <si>
+    <t>Transparencia</t>
+  </si>
+  <si>
+    <t>Responsabilidad social</t>
+  </si>
+  <si>
+    <t>Calidad</t>
+  </si>
+  <si>
+    <t>Honestidad</t>
+  </si>
+  <si>
+    <t>En la medida de lo posible nuestros productos son amigables con el medio ambiente, ya que los compramos siendo hechos con materiales reciclados</t>
+  </si>
+  <si>
+    <t>Nuestra prioridad es la salud del cliente. Todos nuestros procedimientos son honestos con el cliente para certificar la calidad del producto y la felicidad del cliente que lo compró</t>
+  </si>
+  <si>
+    <t>Tenemos la obligación con la comunidad de ser una empresa amable, que se preocupa por el cliente y por sus empleados.</t>
+  </si>
+  <si>
+    <t>Nuestros productos siempre tienen los estándares de calidad más altos, sin excepciones.</t>
+  </si>
+  <si>
+    <t>Como empresa colombiana estamos en la obigacion de contribuir con un porcentaje de nuestras ganancias al estado. De igual manera prohibimos cualquier accion que nos pueda catalogar como competencia desleal</t>
   </si>
 </sst>
 </file>
@@ -506,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ABDEE2F-9DA5-4F4F-A9BF-B9BEA22ACD0E}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -546,13 +582,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.15">
       <c r="A6" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="3" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -561,7 +597,7 @@
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -569,14 +605,18 @@
         <v>8</v>
       </c>
       <c r="B8" s="8"/>
-      <c r="C8" s="3"/>
-    </row>
-    <row r="9" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C8" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="60" x14ac:dyDescent="0.15">
       <c r="A9" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="8"/>
-      <c r="C9" s="3"/>
+      <c r="C9" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="10" spans="1:3" ht="10.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="5"/>
@@ -601,40 +641,60 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.15">
       <c r="A13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="60" x14ac:dyDescent="0.15">
+      <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-    </row>
-    <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.15">
-      <c r="A14" s="3" t="s">
+      <c r="B14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.15">
+      <c r="A15" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-    </row>
-    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.15">
-      <c r="A15" s="3" t="s">
+      <c r="B15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.15">
+      <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-    </row>
-    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.15">
-      <c r="A16" s="3" t="s">
+      <c r="B16" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="60" x14ac:dyDescent="0.15">
+      <c r="A17" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-    </row>
-    <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.15">
-      <c r="A17" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
+      <c r="B17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>